<commit_message>
Working on the muscle scaling
</commit_message>
<xml_diff>
--- a/muscleLab/MuscleMaxForceFromVolumeFraction_PennationAdjusted.xlsx
+++ b/muscleLab/MuscleMaxForceFromVolumeFraction_PennationAdjusted.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silder\Dropbox\DARPA_shared\Model Files and Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repo\stackJimmy\muscleLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,7 +32,7 @@
     <author>Amy Silder</author>
   </authors>
   <commentList>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="H8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="189">
   <si>
     <t>Subject</t>
   </si>
@@ -508,6 +508,126 @@
   </si>
   <si>
     <t>** Taken from Figure 5A, a linear regression in Geoff's paper</t>
+  </si>
+  <si>
+    <t>'addbrev_r'</t>
+  </si>
+  <si>
+    <t>'addlong_r'</t>
+  </si>
+  <si>
+    <t>'addmagDist_r'</t>
+  </si>
+  <si>
+    <t>'addmagIsch_r'</t>
+  </si>
+  <si>
+    <t>'addmagMid_r'</t>
+  </si>
+  <si>
+    <t>'addmagProx_r'</t>
+  </si>
+  <si>
+    <t>'bflh_r'</t>
+  </si>
+  <si>
+    <t>'bfsh_r'</t>
+  </si>
+  <si>
+    <t>'edl_r'</t>
+  </si>
+  <si>
+    <t>'ehl_r'</t>
+  </si>
+  <si>
+    <t>'fdl_r'</t>
+  </si>
+  <si>
+    <t>'fhl_r'</t>
+  </si>
+  <si>
+    <t>'gaslat_r'</t>
+  </si>
+  <si>
+    <t>'gasmed_r'</t>
+  </si>
+  <si>
+    <t>'glmax1_r'</t>
+  </si>
+  <si>
+    <t>'glmax2_r'</t>
+  </si>
+  <si>
+    <t>'glmax3_r'</t>
+  </si>
+  <si>
+    <t>'glmed1_r'</t>
+  </si>
+  <si>
+    <t>'glmed2_r'</t>
+  </si>
+  <si>
+    <t>'glmed3_r'</t>
+  </si>
+  <si>
+    <t>'glmin1_r'</t>
+  </si>
+  <si>
+    <t>'glmin2_r'</t>
+  </si>
+  <si>
+    <t>'glmin3_r'</t>
+  </si>
+  <si>
+    <t>'grac_r'</t>
+  </si>
+  <si>
+    <t>'iliacus_r'</t>
+  </si>
+  <si>
+    <t>'perbrev_r'</t>
+  </si>
+  <si>
+    <t>'perlong_r'</t>
+  </si>
+  <si>
+    <t>'piri_r'</t>
+  </si>
+  <si>
+    <t>'psoas_r'</t>
+  </si>
+  <si>
+    <t>'recfem_r'</t>
+  </si>
+  <si>
+    <t>'sart_r'</t>
+  </si>
+  <si>
+    <t>'semimem_r'</t>
+  </si>
+  <si>
+    <t>'semiten_r'</t>
+  </si>
+  <si>
+    <t>'soleus_r'</t>
+  </si>
+  <si>
+    <t>'tfl_r'</t>
+  </si>
+  <si>
+    <t>'tibant_r'</t>
+  </si>
+  <si>
+    <t>'tibpost_r'</t>
+  </si>
+  <si>
+    <t>'vasint_r'</t>
+  </si>
+  <si>
+    <t>'vaslat_r'</t>
+  </si>
+  <si>
+    <t>'vasmed_r'</t>
   </si>
 </sst>
 </file>
@@ -1556,11 +1676,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="414991208"/>
-        <c:axId val="414991600"/>
+        <c:axId val="138408992"/>
+        <c:axId val="138409552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="414991208"/>
+        <c:axId val="138408992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1570,12 +1690,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="414991600"/>
+        <c:crossAx val="138409552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="414991600"/>
+        <c:axId val="138409552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1586,7 +1706,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="414991208"/>
+        <c:crossAx val="138408992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1846,11 +1966,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="400063072"/>
-        <c:axId val="400063464"/>
+        <c:axId val="138411792"/>
+        <c:axId val="138412352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="400063072"/>
+        <c:axId val="138411792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1860,12 +1980,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="400063464"/>
+        <c:crossAx val="138412352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="400063464"/>
+        <c:axId val="138412352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1876,7 +1996,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="400063072"/>
+        <c:crossAx val="138411792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3201,59 +3321,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S57"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O4"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="7.875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="11.375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.875" style="3" customWidth="1"/>
-    <col min="8" max="9" width="10.375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="10.875" style="3" customWidth="1"/>
-    <col min="11" max="13" width="3" style="13" customWidth="1"/>
-    <col min="14" max="14" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.625" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="10.875" style="4"/>
+    <col min="1" max="2" width="30.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="7.875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.375" style="3" customWidth="1"/>
+    <col min="6" max="7" width="11.375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.875" style="3" customWidth="1"/>
+    <col min="9" max="10" width="10.375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="10.875" style="3" customWidth="1"/>
+    <col min="12" max="14" width="3" style="13" customWidth="1"/>
+    <col min="15" max="15" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.625" style="3" customWidth="1"/>
+    <col min="18" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="63" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="G1" s="3" t="s">
+      <c r="C1" s="24"/>
+      <c r="H1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N2" s="5" t="s">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="O2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="9">
+      <c r="P2" s="9">
         <v>30</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="Q2" s="24" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="C3" s="3" t="s">
         <v>39</v>
       </c>
@@ -3264,34 +3381,34 @@
         <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="H3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="O3" s="9">
+      <c r="P3" s="9">
         <v>75.337000000000003</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="Q3" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="Q3" s="24"/>
       <c r="R3" s="24"/>
       <c r="S3" s="24"/>
-    </row>
-    <row r="4" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T3" s="24"/>
+    </row>
+    <row r="4" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="C4" s="3" t="s">
         <v>44</v>
       </c>
@@ -3302,2027 +3419,2163 @@
         <v>44</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="9">
+      <c r="P4" s="9">
         <v>1.7</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="Q4" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="Q4" s="25"/>
-    </row>
-    <row r="5" spans="1:19" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="R4" s="25"/>
+    </row>
+    <row r="5" spans="1:20" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>52</v>
       </c>
       <c r="G5" s="7" t="s">
         <v>52</v>
       </c>
       <c r="H5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="O5" s="5">
-        <f>47.05*$O$3*$O$4 + 1289.6</f>
+      <c r="P5" s="5">
+        <f>47.05*$P$3*$P$4 + 1289.6</f>
         <v>7315.4299449999999</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="R5" s="3">
         <v>7488.4224599999998</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="8">
         <v>1.47</v>
       </c>
-      <c r="C6" s="3">
-        <f>B6/100*$O$5</f>
+      <c r="D6" s="3">
+        <f>C6/100*$P$5</f>
         <v>107.5368201915</v>
       </c>
-      <c r="D6" s="3">
-        <f>C6/G6</f>
+      <c r="E6" s="3">
+        <f>D6/H6</f>
         <v>10.430341434675071</v>
       </c>
-      <c r="E6" s="7">
-        <f>D6*$O$2</f>
+      <c r="F6" s="7">
+        <f>E6*$P$2</f>
         <v>312.91024304025211</v>
-      </c>
-      <c r="F6" s="8">
-        <v>10.31</v>
       </c>
       <c r="G6" s="8">
         <v>10.31</v>
       </c>
       <c r="H6" s="8">
+        <v>10.31</v>
+      </c>
+      <c r="I6" s="8">
         <v>6.1</v>
       </c>
-      <c r="I6" s="3">
-        <f>H6*PI()/180</f>
+      <c r="J6" s="3">
+        <f>I6*PI()/180</f>
         <v>0.10646508437165408</v>
       </c>
-      <c r="J6" s="8">
+      <c r="K6" s="8">
         <v>3.6</v>
       </c>
-      <c r="O6" s="5">
-        <f>56.933*$O$3*$O$4</f>
+      <c r="P6" s="5">
+        <f>56.933*$P$3*$P$4</f>
         <v>7291.574415699999</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="Q6" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="8">
         <v>2.2599999999999998</v>
       </c>
-      <c r="C7" s="3">
-        <f>B7/100*$O$5</f>
+      <c r="D7" s="3">
+        <f>C7/100*$P$5</f>
         <v>165.328716757</v>
       </c>
-      <c r="D7" s="3">
-        <f>C7/G7</f>
+      <c r="E7" s="3">
+        <f>D7/H7</f>
         <v>15.279918369408502</v>
       </c>
-      <c r="E7" s="7">
-        <f>D7*$O$2</f>
+      <c r="F7" s="7">
+        <f>E7*$P$2</f>
         <v>458.39755108225506</v>
-      </c>
-      <c r="F7" s="8">
-        <v>10.82</v>
       </c>
       <c r="G7" s="8">
         <v>10.82</v>
       </c>
       <c r="H7" s="8">
+        <v>10.82</v>
+      </c>
+      <c r="I7" s="8">
         <v>7.1</v>
       </c>
-      <c r="I7" s="3">
-        <f t="shared" ref="I7:I53" si="0">H7*PI()/180</f>
+      <c r="J7" s="3">
+        <f t="shared" ref="J7:J53" si="0">I7*PI()/180</f>
         <v>0.12391837689159739</v>
       </c>
-      <c r="J7" s="8">
+      <c r="K7" s="8">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8"/>
+      <c r="C8" s="8">
         <v>7.86</v>
       </c>
-      <c r="C8" s="3">
-        <f>B8/100*$O$5</f>
+      <c r="D8" s="3">
+        <f>C8/100*$P$5</f>
         <v>574.99279367700001</v>
       </c>
-      <c r="D8" s="3">
-        <f>C8/G8</f>
+      <c r="E8" s="3">
+        <f>D8/H8</f>
         <v>39.819445545498617</v>
       </c>
-      <c r="E8" s="7">
-        <f>D8*$O$2</f>
+      <c r="F8" s="7">
+        <f>E8*$P$2</f>
         <v>1194.5833663649585</v>
       </c>
-      <c r="G8" s="8">
+      <c r="H8" s="8">
         <v>14.44</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I8" s="8">
         <v>15.5</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <f t="shared" si="0"/>
         <v>0.27052603405912107</v>
       </c>
-      <c r="J8" s="8"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D9" s="10">
-        <f>E9/$O$2</f>
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="10">
+        <f>F9/$P$2</f>
         <v>9.9548613863746542</v>
       </c>
-      <c r="E9" s="7">
-        <f>E8/4</f>
+      <c r="F9" s="7">
+        <f>F8/4</f>
         <v>298.64584159123962</v>
       </c>
-      <c r="F9" s="8">
+      <c r="G9" s="8">
         <v>17.72</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8">
+      <c r="H9" s="8"/>
+      <c r="I9" s="8">
         <v>13.8</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <f t="shared" si="0"/>
         <v>0.24085543677521748</v>
       </c>
-      <c r="J9" s="8">
+      <c r="K9" s="8">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="10">
-        <f t="shared" ref="D10:D12" si="1">E10/$O$2</f>
+      <c r="B10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" ref="E10:E12" si="1">F10/$P$2</f>
         <v>9.9548613863746542</v>
       </c>
-      <c r="E10" s="7">
-        <f>E8/4</f>
+      <c r="F10" s="7">
+        <f>F8/4</f>
         <v>298.64584159123962</v>
       </c>
-      <c r="F10" s="8">
+      <c r="G10" s="8">
         <v>15.62</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8">
+      <c r="H10" s="8"/>
+      <c r="I10" s="8">
         <v>11.9</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <f t="shared" si="0"/>
         <v>0.2076941809873252</v>
       </c>
-      <c r="J10" s="8">
+      <c r="K10" s="8">
         <v>22.1</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="10">
+      <c r="B11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="10">
         <f t="shared" si="1"/>
         <v>9.9548613863746542</v>
       </c>
-      <c r="E11" s="7">
-        <f>E8/4</f>
+      <c r="F11" s="7">
+        <f>F8/4</f>
         <v>298.64584159123962</v>
       </c>
-      <c r="F11" s="8">
+      <c r="G11" s="8">
         <v>13.77</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8">
+      <c r="H11" s="8"/>
+      <c r="I11" s="8">
         <v>14.7</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <f t="shared" si="0"/>
         <v>0.25656340004316641</v>
       </c>
-      <c r="J11" s="8">
+      <c r="K11" s="8">
         <v>4.8</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="10">
+      <c r="B12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="10">
         <f t="shared" si="1"/>
         <v>9.9548613863746542</v>
       </c>
-      <c r="E12" s="7">
-        <f>E8/4</f>
+      <c r="F12" s="7">
+        <f>F8/4</f>
         <v>298.64584159123962</v>
       </c>
-      <c r="F12" s="8">
+      <c r="G12" s="8">
         <v>10.56</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8">
+      <c r="H12" s="8"/>
+      <c r="I12" s="8">
         <v>22.2</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <f t="shared" si="0"/>
         <v>0.38746309394274114</v>
       </c>
-      <c r="J12" s="8">
+      <c r="K12" s="8">
         <v>4.3</v>
       </c>
-      <c r="N12" s="15" t="s">
+      <c r="O12" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="O12" s="7" t="s">
+      <c r="P12" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="P12" s="7" t="s">
+      <c r="Q12" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="Q12" s="7" t="s">
+      <c r="R12" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="8">
         <v>2.92</v>
       </c>
-      <c r="C13" s="3">
-        <f t="shared" ref="C13:C21" si="2">B13/100*$O$5</f>
+      <c r="D13" s="3">
+        <f t="shared" ref="D13:D21" si="2">C13/100*$P$5</f>
         <v>213.61055439399999</v>
       </c>
-      <c r="D13" s="3">
-        <f t="shared" ref="D13:D20" si="3">C13/G13</f>
+      <c r="E13" s="3">
+        <f t="shared" ref="E13:E20" si="3">D13/H13</f>
         <v>21.886327294467211</v>
       </c>
-      <c r="E13" s="7">
-        <f t="shared" ref="E13:E22" si="4">D13*$O$2</f>
+      <c r="F13" s="7">
+        <f t="shared" ref="F13:F22" si="4">E13*$P$2</f>
         <v>656.58981883401634</v>
-      </c>
-      <c r="F13" s="8">
-        <v>9.76</v>
       </c>
       <c r="G13" s="8">
         <v>9.76</v>
       </c>
       <c r="H13" s="8">
+        <v>9.76</v>
+      </c>
+      <c r="I13" s="8">
         <v>11.6</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <f t="shared" si="0"/>
         <v>0.20245819323134223</v>
       </c>
-      <c r="J13" s="8">
+      <c r="K13" s="8">
         <v>32.200000000000003</v>
       </c>
-      <c r="N13" s="12" t="s">
+      <c r="O13" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="O13" s="12">
+      <c r="P13" s="12">
         <v>6.93</v>
       </c>
-      <c r="P13" s="12">
+      <c r="Q13" s="12">
         <v>5.7</v>
       </c>
-      <c r="Q13" s="4">
-        <f>O13*P13</f>
+      <c r="R13" s="4">
+        <f>P13*Q13</f>
         <v>39.500999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" s="8">
         <v>1.4</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="3">
         <f t="shared" si="2"/>
         <v>102.41601922999999</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <f t="shared" si="3"/>
         <v>9.2852238649138705</v>
       </c>
-      <c r="E14" s="7">
-        <f>D14*$O$2</f>
+      <c r="F14" s="7">
+        <f>E14*$P$2</f>
         <v>278.55671594741614</v>
-      </c>
-      <c r="F14" s="8">
-        <v>11.03</v>
       </c>
       <c r="G14" s="8">
         <v>11.03</v>
       </c>
       <c r="H14" s="8">
+        <v>11.03</v>
+      </c>
+      <c r="I14" s="8">
         <v>12.3</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <f t="shared" si="0"/>
         <v>0.21467549799530256</v>
       </c>
-      <c r="J14" s="8">
+      <c r="K14" s="8">
         <v>10.4</v>
       </c>
-      <c r="N14" s="12" t="s">
+      <c r="O14" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="O14" s="12">
+      <c r="P14" s="12">
         <v>7.48</v>
       </c>
-      <c r="P14" s="12">
+      <c r="Q14" s="12">
         <v>2.7</v>
       </c>
-      <c r="Q14" s="4">
-        <f t="shared" ref="Q14:Q15" si="5">O14*P14</f>
+      <c r="R14" s="4">
+        <f t="shared" ref="R14:R15" si="5">P14*Q14</f>
         <v>20.196000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="10">
-        <f>1.44*(Q13/SUM($Q$13:$Q$15))</f>
+      <c r="B15" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" s="10">
+        <f>1.44*(R13/SUM($R$13:$R$15))</f>
         <v>0.79718651070173863</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="3">
         <f t="shared" si="2"/>
         <v>58.317620721375611</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <f t="shared" si="3"/>
         <v>8.4152410853355857</v>
       </c>
-      <c r="E15" s="7">
+      <c r="F15" s="7">
         <f t="shared" si="4"/>
         <v>252.45723256006758</v>
       </c>
-      <c r="F15" s="8">
-        <v>6.93</v>
-      </c>
       <c r="G15" s="8">
         <v>6.93</v>
       </c>
       <c r="H15" s="8">
+        <v>6.93</v>
+      </c>
+      <c r="I15" s="8">
         <v>10.8</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <f t="shared" si="0"/>
         <v>0.18849555921538758</v>
       </c>
-      <c r="J15" s="8">
+      <c r="K15" s="8">
         <v>36.700000000000003</v>
       </c>
-      <c r="N15" s="12" t="s">
+      <c r="O15" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="O15" s="12">
+      <c r="P15" s="12">
         <v>7.9</v>
       </c>
-      <c r="P15" s="12">
+      <c r="Q15" s="12">
         <f>90/61</f>
         <v>1.4754098360655739</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="R15" s="4">
         <f t="shared" si="5"/>
         <v>11.655737704918034</v>
       </c>
-      <c r="R15" s="4" t="s">
+      <c r="S15" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="10">
-        <f>1.44*(Q14/SUM($Q$13:$Q$15))</f>
+      <c r="B16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" s="10">
+        <f>1.44*(R14/SUM($R$13:$R$15))</f>
         <v>0.40758408065953555</v>
       </c>
-      <c r="C16" s="3">
+      <c r="D16" s="3">
         <f t="shared" si="2"/>
         <v>29.816527887620616</v>
       </c>
-      <c r="D16" s="3">
+      <c r="E16" s="3">
         <f t="shared" si="3"/>
         <v>3.986166829895804</v>
       </c>
-      <c r="E16" s="7">
+      <c r="F16" s="7">
         <f t="shared" si="4"/>
         <v>119.58500489687412</v>
       </c>
-      <c r="F16" s="8">
-        <v>7.48</v>
-      </c>
       <c r="G16" s="8">
         <v>7.48</v>
       </c>
       <c r="H16" s="8">
+        <v>7.48</v>
+      </c>
+      <c r="I16" s="8">
         <v>9.4</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <f t="shared" si="0"/>
         <v>0.16406094968746698</v>
       </c>
-      <c r="J16" s="8">
+      <c r="K16" s="8">
         <v>33.200000000000003</v>
       </c>
-      <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q16" s="12"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="8">
         <v>0.43</v>
       </c>
-      <c r="C17" s="3">
+      <c r="D17" s="3">
         <f t="shared" si="2"/>
         <v>31.456348763499999</v>
       </c>
-      <c r="D17" s="3">
+      <c r="E17" s="3">
         <f t="shared" si="3"/>
         <v>7.0529929963004481</v>
       </c>
-      <c r="E17" s="7">
+      <c r="F17" s="7">
         <f t="shared" si="4"/>
         <v>211.58978988901345</v>
       </c>
-      <c r="F17" s="8">
-        <v>4.46</v>
-      </c>
       <c r="G17" s="8">
         <v>4.46</v>
       </c>
       <c r="H17" s="8">
+        <v>4.46</v>
+      </c>
+      <c r="I17" s="8">
         <v>13.6</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <f t="shared" si="0"/>
         <v>0.23736477827122882</v>
       </c>
-      <c r="J17" s="8">
+      <c r="K17" s="8">
         <v>37.799999999999997</v>
       </c>
-      <c r="N17" s="12" t="s">
+      <c r="O17" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="O17" s="12">
+      <c r="P17" s="12">
         <v>14.7</v>
       </c>
-      <c r="P17" s="12">
+      <c r="Q17" s="12">
         <f>546.1/61</f>
         <v>8.9524590163934423</v>
       </c>
-      <c r="Q17" s="4">
-        <f>O17*P17</f>
+      <c r="R17" s="4">
+        <f>P17*Q17</f>
         <v>131.60114754098359</v>
       </c>
-      <c r="R17" s="4" t="s">
+      <c r="S17" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" s="8">
         <v>1.0900000000000001</v>
       </c>
-      <c r="C18" s="3">
+      <c r="D18" s="3">
         <f t="shared" si="2"/>
         <v>79.738186400499998</v>
       </c>
-      <c r="D18" s="3">
+      <c r="E18" s="3">
         <f t="shared" si="3"/>
         <v>15.130585654743834</v>
       </c>
-      <c r="E18" s="7">
+      <c r="F18" s="7">
         <f t="shared" si="4"/>
         <v>453.91756964231502</v>
       </c>
-      <c r="F18" s="8">
-        <v>5.27</v>
-      </c>
       <c r="G18" s="8">
         <v>5.27</v>
       </c>
       <c r="H18" s="8">
+        <v>5.27</v>
+      </c>
+      <c r="I18" s="8">
         <v>16.899999999999999</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <f t="shared" si="0"/>
         <v>0.29496064358704166</v>
       </c>
-      <c r="J18" s="8">
+      <c r="K18" s="8">
         <v>35.6</v>
       </c>
-      <c r="N18" s="12" t="s">
+      <c r="O18" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="O18" s="12">
+      <c r="P18" s="12">
         <v>15.7</v>
       </c>
-      <c r="P18" s="12">
+      <c r="Q18" s="12">
         <f>780.5/61</f>
         <v>12.795081967213115</v>
       </c>
-      <c r="Q18" s="4">
-        <f t="shared" ref="Q18:Q30" si="6">O18*P18</f>
+      <c r="R18" s="4">
+        <f t="shared" ref="R18:R30" si="6">P18*Q18</f>
         <v>200.88278688524588</v>
       </c>
-      <c r="R18" s="4" t="s">
+      <c r="S18" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="8">
         <v>2.11</v>
       </c>
-      <c r="C19" s="3">
+      <c r="D19" s="3">
         <f t="shared" si="2"/>
         <v>154.35557183949999</v>
       </c>
-      <c r="D19" s="3">
+      <c r="E19" s="3">
         <f t="shared" si="3"/>
         <v>26.2509475917517</v>
       </c>
-      <c r="E19" s="7">
+      <c r="F19" s="7">
         <f t="shared" si="4"/>
         <v>787.52842775255101</v>
       </c>
-      <c r="F19" s="8">
-        <v>5.88</v>
-      </c>
       <c r="G19" s="8">
         <v>5.88</v>
       </c>
       <c r="H19" s="8">
+        <v>5.88</v>
+      </c>
+      <c r="I19" s="8">
         <v>12</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <f t="shared" si="0"/>
         <v>0.20943951023931953</v>
       </c>
-      <c r="J19" s="8">
+      <c r="K19" s="8">
         <v>38.200000000000003</v>
       </c>
-      <c r="N19" s="12" t="s">
+      <c r="O19" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="O19" s="12">
+      <c r="P19" s="12">
         <v>16.7</v>
       </c>
-      <c r="P19" s="12">
+      <c r="Q19" s="12">
         <f>526.1/61</f>
         <v>8.6245901639344265</v>
       </c>
-      <c r="Q19" s="4">
+      <c r="R19" s="4">
         <f t="shared" si="6"/>
         <v>144.0306557377049</v>
       </c>
-      <c r="R19" s="4" t="s">
+      <c r="S19" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C20" s="8">
         <v>3.62</v>
       </c>
-      <c r="C20" s="3">
+      <c r="D20" s="3">
         <f t="shared" si="2"/>
         <v>264.818564009</v>
       </c>
-      <c r="D20" s="3">
+      <c r="E20" s="3">
         <f t="shared" si="3"/>
         <v>51.925208629215689</v>
       </c>
-      <c r="E20" s="7">
+      <c r="F20" s="7">
         <f t="shared" si="4"/>
         <v>1557.7562588764706</v>
       </c>
-      <c r="F20" s="8">
-        <v>5.0999999999999996</v>
-      </c>
       <c r="G20" s="8">
         <v>5.0999999999999996</v>
       </c>
       <c r="H20" s="8">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I20" s="8">
         <v>9.9</v>
       </c>
-      <c r="I20" s="3">
+      <c r="J20" s="3">
         <f t="shared" si="0"/>
         <v>0.17278759594743864</v>
       </c>
-      <c r="J20" s="8">
+      <c r="K20" s="8">
         <v>40.1</v>
       </c>
-      <c r="N20" s="12"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q20" s="12"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21"/>
+      <c r="C21" s="10">
         <v>0.23</v>
       </c>
-      <c r="C21" s="3">
+      <c r="D21" s="3">
         <f t="shared" si="2"/>
         <v>16.825488873499999</v>
       </c>
-      <c r="D21" s="3">
-        <f>C21/F21</f>
+      <c r="E21" s="3">
+        <f>D21/G21</f>
         <v>7.0106203639583331</v>
       </c>
-      <c r="E21" s="7">
+      <c r="F21" s="7">
         <f t="shared" si="4"/>
         <v>210.31861091874998</v>
       </c>
-      <c r="F21" s="8">
+      <c r="G21" s="8">
         <v>2.4</v>
       </c>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8">
+      <c r="H21" s="8"/>
+      <c r="I21" s="8">
         <v>0</v>
       </c>
-      <c r="I21" s="3">
+      <c r="J21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J21" s="8">
+      <c r="K21" s="8">
         <v>3.9</v>
       </c>
-      <c r="N21" s="12" t="s">
+      <c r="O21" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="O21" s="12">
+      <c r="P21" s="12">
         <v>7.3</v>
       </c>
-      <c r="P21" s="12">
+      <c r="Q21" s="12">
         <f>881.1/61</f>
         <v>14.444262295081968</v>
       </c>
-      <c r="Q21" s="4">
+      <c r="R21" s="4">
         <f t="shared" si="6"/>
         <v>105.44311475409836</v>
       </c>
-      <c r="R21" s="4" t="s">
+      <c r="S21" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22"/>
+      <c r="C22" s="8">
         <v>11.93</v>
       </c>
-      <c r="C22" s="3">
-        <f>B22/100*$O$5</f>
+      <c r="D22" s="3">
+        <f>C22/100*$P$5</f>
         <v>872.73079243849998</v>
       </c>
-      <c r="D22" s="3">
-        <f>C22/G22</f>
+      <c r="E22" s="3">
+        <f>D22/H22</f>
         <v>55.623377465806243</v>
       </c>
-      <c r="E22" s="7">
+      <c r="F22" s="7">
         <f t="shared" si="4"/>
         <v>1668.7013239741873</v>
       </c>
-      <c r="G22" s="8">
+      <c r="H22" s="8">
         <v>15.69</v>
       </c>
-      <c r="H22" s="8">
+      <c r="I22" s="8">
         <v>21.9</v>
       </c>
-      <c r="I22" s="3">
+      <c r="J22" s="3">
         <f t="shared" si="0"/>
         <v>0.38222710618675809</v>
       </c>
-      <c r="J22" s="8"/>
-      <c r="N22" s="12" t="s">
+      <c r="K22" s="8"/>
+      <c r="O22" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="O22" s="12">
+      <c r="P22" s="12">
         <v>7.3</v>
       </c>
-      <c r="P22" s="12">
+      <c r="Q22" s="12">
         <f>616.5/61</f>
         <v>10.10655737704918</v>
       </c>
-      <c r="Q22" s="4">
+      <c r="R22" s="4">
         <f t="shared" si="6"/>
         <v>73.777868852459008</v>
       </c>
-      <c r="R22" s="4" t="s">
+      <c r="S22" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="10">
-        <f>$B$22*Q17/SUM($Q$17:$Q$19)</f>
+      <c r="B23" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="10">
+        <f>$C$22*R17/SUM($R$17:$R$19)</f>
         <v>3.2947610053740632</v>
       </c>
-      <c r="C23" s="3">
-        <f>B23/100*$O$5</f>
+      <c r="D23" s="3">
+        <f>C23/100*$P$5</f>
         <v>241.02593320331727</v>
       </c>
-      <c r="D23" s="14">
-        <f>C23/F23</f>
+      <c r="E23" s="14">
+        <f>D23/G23</f>
         <v>16.396321986620222</v>
       </c>
-      <c r="E23" s="7">
-        <f>D23*$O$2</f>
+      <c r="F23" s="7">
+        <f>E23*$P$2</f>
         <v>491.88965959860667</v>
       </c>
-      <c r="F23" s="8">
+      <c r="G23" s="8">
         <v>14.7</v>
       </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8">
+      <c r="H23" s="8"/>
+      <c r="I23" s="8">
         <v>21.1</v>
       </c>
-      <c r="I23" s="3">
+      <c r="J23" s="3">
         <f t="shared" si="0"/>
         <v>0.36826447217080355</v>
       </c>
-      <c r="J23" s="8">
+      <c r="K23" s="8">
         <v>5</v>
       </c>
-      <c r="N23" s="12" t="s">
+      <c r="O23" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="O23" s="12">
+      <c r="P23" s="12">
         <v>7.3</v>
       </c>
-      <c r="P23" s="12">
+      <c r="Q23" s="12">
         <f>702/61</f>
         <v>11.508196721311476</v>
       </c>
-      <c r="Q23" s="4">
+      <c r="R23" s="4">
         <f t="shared" si="6"/>
         <v>84.009836065573779</v>
       </c>
-      <c r="R23" s="4" t="s">
+      <c r="S23" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="10">
-        <f t="shared" ref="B24:B25" si="7">$B$22*Q18/SUM($Q$17:$Q$19)</f>
+      <c r="B24" t="s">
+        <v>164</v>
+      </c>
+      <c r="C24" s="10">
+        <f t="shared" ref="C24:C25" si="7">$C$22*R18/SUM($R$17:$R$19)</f>
         <v>5.0292933249252849</v>
       </c>
-      <c r="C24" s="3">
-        <f t="shared" ref="C24:C25" si="8">B24/100*$O$5</f>
+      <c r="D24" s="3">
+        <f t="shared" ref="D24:D25" si="8">C24/100*$P$5</f>
         <v>367.91442991347049</v>
       </c>
-      <c r="D24" s="14">
-        <f t="shared" ref="D24:D25" si="9">C24/F24</f>
+      <c r="E24" s="14">
+        <f t="shared" ref="E24:E25" si="9">D24/G24</f>
         <v>23.434040121877104</v>
       </c>
-      <c r="E24" s="7">
-        <f t="shared" ref="E24:E25" si="10">D24*$O$2</f>
+      <c r="F24" s="7">
+        <f t="shared" ref="F24:F25" si="10">E24*$P$2</f>
         <v>703.02120365631311</v>
       </c>
-      <c r="F24" s="8">
+      <c r="G24" s="8">
         <v>15.7</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8">
+      <c r="H24" s="8"/>
+      <c r="I24" s="8">
         <v>21.9</v>
       </c>
-      <c r="I24" s="3">
+      <c r="J24" s="3">
         <f t="shared" si="0"/>
         <v>0.38222710618675809</v>
       </c>
-      <c r="J24" s="8">
+      <c r="K24" s="8">
         <v>7.3</v>
       </c>
-      <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q24" s="12"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C25" s="10">
         <f t="shared" si="7"/>
         <v>3.6059456697006507</v>
       </c>
-      <c r="C25" s="3">
+      <c r="D25" s="3">
         <f t="shared" si="8"/>
         <v>263.79042932171217</v>
       </c>
-      <c r="D25" s="14">
+      <c r="E25" s="14">
         <f t="shared" si="9"/>
         <v>15.79583409112049</v>
       </c>
-      <c r="E25" s="7">
+      <c r="F25" s="7">
         <f t="shared" si="10"/>
         <v>473.87502273361468</v>
       </c>
-      <c r="F25" s="8">
+      <c r="G25" s="8">
         <v>16.7</v>
       </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8">
+      <c r="H25" s="8"/>
+      <c r="I25" s="8">
         <v>22.8</v>
       </c>
-      <c r="I25" s="3">
+      <c r="J25" s="3">
         <f t="shared" si="0"/>
         <v>0.39793506945470719</v>
       </c>
-      <c r="J25" s="8">
+      <c r="K25" s="8">
         <v>7</v>
       </c>
-      <c r="N25" s="12" t="s">
+      <c r="O25" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="O25" s="3">
+      <c r="P25" s="3">
         <v>6.8</v>
       </c>
-      <c r="P25" s="12">
+      <c r="Q25" s="12">
         <f>180/61</f>
         <v>2.9508196721311477</v>
       </c>
-      <c r="Q25" s="4">
+      <c r="R25" s="4">
         <f t="shared" si="6"/>
         <v>20.065573770491802</v>
       </c>
-      <c r="R25" s="4" t="s">
+      <c r="S25" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="8">
+      <c r="B26"/>
+      <c r="C26" s="8">
         <v>4.54</v>
       </c>
-      <c r="C26" s="3">
-        <f>B26/100*$O$5</f>
+      <c r="D26" s="3">
+        <f>C26/100*$P$5</f>
         <v>332.12051950300003</v>
       </c>
-      <c r="D26" s="3">
-        <f>C26/G26</f>
+      <c r="E26" s="3">
+        <f>D26/H26</f>
         <v>45.309757094542974</v>
       </c>
-      <c r="E26" s="7">
-        <f>D26*$O$2</f>
+      <c r="F26" s="7">
+        <f>E26*$P$2</f>
         <v>1359.2927128362892</v>
       </c>
-      <c r="G26" s="8">
+      <c r="H26" s="8">
         <v>7.33</v>
       </c>
-      <c r="H26" s="8">
+      <c r="I26" s="8">
         <v>20.5</v>
       </c>
-      <c r="I26" s="3">
+      <c r="J26" s="3">
         <f t="shared" si="0"/>
         <v>0.3577924966588375</v>
       </c>
-      <c r="J26" s="8"/>
-      <c r="N26" s="12" t="s">
+      <c r="K26" s="8"/>
+      <c r="O26" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="O26" s="3">
+      <c r="P26" s="3">
         <v>5.6</v>
       </c>
-      <c r="P26" s="12">
+      <c r="Q26" s="12">
         <f>190/61</f>
         <v>3.1147540983606556</v>
       </c>
-      <c r="Q26" s="4">
+      <c r="R26" s="4">
         <f t="shared" si="6"/>
         <v>17.442622950819672</v>
       </c>
-      <c r="R26" s="4" t="s">
+      <c r="S26" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="10">
-        <f>$B$26*Q21/SUM($Q$21:$Q$23)</f>
+      <c r="B27" t="s">
+        <v>166</v>
+      </c>
+      <c r="C27" s="10">
+        <f>$C$26*R21/SUM($R$21:$R$23)</f>
         <v>1.8186006546644846</v>
       </c>
-      <c r="C27" s="3">
-        <f>B27/100*$O$5</f>
+      <c r="D27" s="3">
+        <f>C27/100*$P$5</f>
         <v>133.03845687129174</v>
       </c>
-      <c r="D27" s="3">
-        <f>C27/F27</f>
+      <c r="E27" s="3">
+        <f>D27/G27</f>
         <v>18.224446146752292</v>
       </c>
-      <c r="E27" s="7">
-        <f>D27*$O$2</f>
+      <c r="F27" s="7">
+        <f>E27*$P$2</f>
         <v>546.73338440256873</v>
       </c>
-      <c r="F27" s="8">
+      <c r="G27" s="8">
         <v>7.3</v>
       </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8">
+      <c r="H27" s="8"/>
+      <c r="I27" s="8">
         <v>20.5</v>
       </c>
-      <c r="I27" s="3">
+      <c r="J27" s="3">
         <f t="shared" si="0"/>
         <v>0.3577924966588375</v>
       </c>
-      <c r="J27" s="8">
+      <c r="K27" s="8">
         <v>5.7</v>
       </c>
-      <c r="N27" s="12" t="s">
+      <c r="O27" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="O27" s="3">
+      <c r="P27" s="3">
         <v>3.8</v>
       </c>
-      <c r="P27" s="12">
+      <c r="Q27" s="12">
         <f>215/61</f>
         <v>3.5245901639344264</v>
       </c>
-      <c r="Q27" s="4">
+      <c r="R27" s="4">
         <f t="shared" si="6"/>
         <v>13.39344262295082</v>
       </c>
-      <c r="R27" s="4" t="s">
+      <c r="S27" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="10">
-        <f t="shared" ref="B28:B29" si="11">$B$26*Q22/SUM($Q$21:$Q$23)</f>
+      <c r="B28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" s="10">
+        <f t="shared" ref="C28:C29" si="11">$C$26*R22/SUM($R$21:$R$23)</f>
         <v>1.2724631751227495</v>
       </c>
-      <c r="C28" s="3">
-        <f t="shared" ref="C28:C29" si="12">B28/100*$O$5</f>
+      <c r="D28" s="3">
+        <f t="shared" ref="D28:D29" si="12">C28/100*$P$5</f>
         <v>93.08615215202741</v>
       </c>
-      <c r="D28" s="3">
-        <f t="shared" ref="D28:D29" si="13">C28/F28</f>
+      <c r="E28" s="3">
+        <f t="shared" ref="E28:E29" si="13">D28/G28</f>
         <v>12.75152769205855</v>
       </c>
-      <c r="E28" s="7">
-        <f t="shared" ref="E28:E29" si="14">D28*$O$2</f>
+      <c r="F28" s="7">
+        <f t="shared" ref="F28:F29" si="14">E28*$P$2</f>
         <v>382.54583076175652</v>
       </c>
-      <c r="F28" s="8">
+      <c r="G28" s="8">
         <v>7.3</v>
       </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8">
+      <c r="H28" s="8"/>
+      <c r="I28" s="8">
         <v>20.5</v>
       </c>
-      <c r="I28" s="3">
+      <c r="J28" s="3">
         <f t="shared" si="0"/>
         <v>0.3577924966588375</v>
       </c>
-      <c r="J28" s="8">
+      <c r="K28" s="8">
         <v>6.6</v>
       </c>
-      <c r="N28" s="12"/>
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q28" s="12"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" s="10">
         <f t="shared" si="11"/>
         <v>1.4489361702127661</v>
       </c>
-      <c r="C29" s="3">
+      <c r="D29" s="3">
         <f t="shared" si="12"/>
         <v>105.99591047968086</v>
       </c>
-      <c r="D29" s="3">
+      <c r="E29" s="3">
         <f t="shared" si="13"/>
         <v>14.519987736942584</v>
       </c>
-      <c r="E29" s="7">
+      <c r="F29" s="7">
         <f t="shared" si="14"/>
         <v>435.59963210827749</v>
       </c>
-      <c r="F29" s="8">
+      <c r="G29" s="8">
         <v>7.3</v>
       </c>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8">
+      <c r="H29" s="8"/>
+      <c r="I29" s="8">
         <v>20.5</v>
       </c>
-      <c r="I29" s="3">
+      <c r="J29" s="3">
         <f t="shared" si="0"/>
         <v>0.3577924966588375</v>
       </c>
-      <c r="J29" s="8">
+      <c r="K29" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="N29" s="12" t="s">
+      <c r="O29" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="O29" s="12">
+      <c r="P29" s="12">
         <v>4.54</v>
       </c>
-      <c r="P29" s="12">
+      <c r="Q29" s="12">
         <v>5</v>
       </c>
-      <c r="Q29" s="4">
+      <c r="R29" s="4">
         <f t="shared" si="6"/>
         <v>22.7</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="8">
+      <c r="B30"/>
+      <c r="C30" s="8">
         <v>1.47</v>
       </c>
-      <c r="C30" s="3">
-        <f>B30/100*$O$5</f>
+      <c r="D30" s="3">
+        <f>C30/100*$P$5</f>
         <v>107.5368201915</v>
       </c>
-      <c r="E30" s="7"/>
-      <c r="G30" s="8"/>
+      <c r="F30" s="7"/>
       <c r="H30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="N30" s="12" t="s">
+      <c r="I30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="O30" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="O30" s="12">
+      <c r="P30" s="12">
         <v>5.08</v>
       </c>
-      <c r="P30" s="12">
+      <c r="Q30" s="12">
         <v>10.7</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="R30" s="4">
         <f t="shared" si="6"/>
         <v>54.355999999999995</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="10">
-        <f>$B$30*Q25/SUM($Q$25:$Q$27)</f>
+      <c r="B31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="10">
+        <f>$C$30*R25/SUM($R$25:$R$27)</f>
         <v>0.57947826086956511</v>
       </c>
-      <c r="C31" s="3">
-        <f>B31/100*$O$5</f>
+      <c r="D31" s="3">
+        <f>C31/100*$P$5</f>
         <v>42.391326220417383</v>
       </c>
-      <c r="D31" s="3">
-        <f>C31/F31</f>
+      <c r="E31" s="3">
+        <f>D31/G31</f>
         <v>6.2340185618260859</v>
       </c>
-      <c r="E31" s="7">
-        <f t="shared" ref="E31:E39" si="15">D31*$O$2</f>
+      <c r="F31" s="7">
+        <f t="shared" ref="F31:F39" si="15">E31*$P$2</f>
         <v>187.02055685478257</v>
-      </c>
-      <c r="F31" s="8">
-        <v>6.8</v>
       </c>
       <c r="G31" s="8">
         <v>6.8</v>
       </c>
       <c r="H31" s="8">
+        <v>6.8</v>
+      </c>
+      <c r="I31" s="8">
         <v>10</v>
       </c>
-      <c r="I31" s="3">
+      <c r="J31" s="3">
         <f t="shared" si="0"/>
         <v>0.17453292519943295</v>
       </c>
-      <c r="J31" s="8">
+      <c r="K31" s="8">
         <v>1.6</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="10">
-        <f t="shared" ref="B32:B33" si="16">$B$30*Q26/SUM($Q$25:$Q$27)</f>
+      <c r="B32" t="s">
+        <v>170</v>
+      </c>
+      <c r="C32" s="10">
+        <f t="shared" ref="C32:C33" si="16">$C$30*R26/SUM($R$25:$R$27)</f>
         <v>0.50372946859903378</v>
       </c>
-      <c r="C32" s="3">
-        <f t="shared" ref="C32:C33" si="17">B32/100*$O$5</f>
+      <c r="D32" s="3">
+        <f t="shared" ref="D32:D33" si="17">C32/100*$P$5</f>
         <v>36.849976387683085</v>
       </c>
-      <c r="D32" s="3">
-        <f>C32/F32</f>
+      <c r="E32" s="3">
+        <f>D32/G32</f>
         <v>6.5803529263719795</v>
       </c>
-      <c r="E32" s="7">
+      <c r="F32" s="7">
         <f t="shared" si="15"/>
         <v>197.4105877911594</v>
       </c>
-      <c r="F32" s="8">
-        <v>5.6</v>
-      </c>
       <c r="G32" s="8">
         <v>5.6</v>
       </c>
       <c r="H32" s="8">
+        <v>5.6</v>
+      </c>
+      <c r="I32" s="8">
         <v>0</v>
       </c>
-      <c r="I32" s="3">
+      <c r="J32" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J32" s="8">
+      <c r="K32" s="8">
         <v>2.6</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B33" s="10">
+      <c r="B33" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33" s="10">
         <f t="shared" si="16"/>
         <v>0.38679227053140092</v>
       </c>
-      <c r="C33" s="3">
+      <c r="D33" s="3">
         <f t="shared" si="17"/>
         <v>28.295517583399512</v>
       </c>
-      <c r="D33" s="3">
-        <f>C33/F33</f>
+      <c r="E33" s="3">
+        <f>D33/G33</f>
         <v>7.446188837736714</v>
       </c>
-      <c r="E33" s="7">
+      <c r="F33" s="7">
         <f t="shared" si="15"/>
         <v>223.38566513210142</v>
       </c>
-      <c r="F33" s="8">
-        <v>3.8</v>
-      </c>
       <c r="G33" s="8">
         <v>3.8</v>
       </c>
       <c r="H33" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="I33" s="8">
         <v>1</v>
       </c>
-      <c r="I33" s="3">
+      <c r="J33" s="3">
         <f t="shared" si="0"/>
         <v>1.7453292519943295E-2</v>
       </c>
-      <c r="J33" s="8">
+      <c r="K33" s="8">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B34" s="8">
+      <c r="B34" t="s">
+        <v>172</v>
+      </c>
+      <c r="C34" s="8">
         <v>1.46</v>
       </c>
-      <c r="C34" s="3">
-        <f t="shared" ref="C34:C39" si="18">B34/100*$O$5</f>
+      <c r="D34" s="3">
+        <f t="shared" ref="D34:D39" si="18">C34/100*$P$5</f>
         <v>106.805277197</v>
       </c>
-      <c r="D34" s="3">
-        <f t="shared" ref="D34:D39" si="19">C34/G34</f>
+      <c r="E34" s="3">
+        <f t="shared" ref="E34:E39" si="19">D34/H34</f>
         <v>4.688554749648814</v>
       </c>
-      <c r="E34" s="7">
+      <c r="F34" s="7">
         <f t="shared" si="15"/>
         <v>140.65664248946442</v>
       </c>
-      <c r="F34" s="8">
-        <v>22.78</v>
-      </c>
       <c r="G34" s="8">
         <v>22.78</v>
       </c>
       <c r="H34" s="8">
+        <v>22.78</v>
+      </c>
+      <c r="I34" s="8">
         <v>8.1999999999999993</v>
       </c>
-      <c r="I34" s="3">
+      <c r="J34" s="3">
         <f t="shared" si="0"/>
         <v>0.143116998663535</v>
       </c>
-      <c r="J34" s="8">
+      <c r="K34" s="8">
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="8">
+      <c r="B35" t="s">
+        <v>173</v>
+      </c>
+      <c r="C35" s="8">
         <v>2.48</v>
       </c>
-      <c r="C35" s="3">
+      <c r="D35" s="3">
         <f t="shared" si="18"/>
         <v>181.42266263599998</v>
       </c>
-      <c r="D35" s="3">
+      <c r="E35" s="3">
         <f t="shared" si="19"/>
         <v>17.019011504315195</v>
       </c>
-      <c r="E35" s="7">
+      <c r="F35" s="7">
         <f t="shared" si="15"/>
         <v>510.57034512945586</v>
       </c>
-      <c r="F35" s="8">
-        <v>10.66</v>
-      </c>
       <c r="G35" s="8">
         <v>10.66</v>
       </c>
       <c r="H35" s="8">
+        <v>10.66</v>
+      </c>
+      <c r="I35" s="8">
         <v>14.3</v>
       </c>
-      <c r="I35" s="3">
+      <c r="J35" s="3">
         <f t="shared" si="0"/>
         <v>0.24958208303518914</v>
       </c>
-      <c r="J35" s="8">
+      <c r="K35" s="8">
         <v>9.4</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="8">
+      <c r="B36"/>
+      <c r="C36" s="8">
         <v>0.92</v>
       </c>
-      <c r="C36" s="3">
+      <c r="D36" s="3">
         <f t="shared" si="18"/>
         <v>67.301955493999998</v>
       </c>
-      <c r="D36" s="3">
+      <c r="E36" s="3">
         <f t="shared" si="19"/>
         <v>5.0602974055639089</v>
       </c>
-      <c r="E36" s="7">
+      <c r="F36" s="7">
         <f t="shared" si="15"/>
         <v>151.80892216691726</v>
       </c>
-      <c r="F36" s="8">
-        <v>13.3</v>
-      </c>
       <c r="G36" s="8">
         <v>13.3</v>
       </c>
       <c r="H36" s="8">
+        <v>13.3</v>
+      </c>
+      <c r="I36" s="8">
         <v>0</v>
       </c>
-      <c r="I36" s="3">
+      <c r="J36" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J36" s="8">
+      <c r="K36" s="8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B37" s="10">
-        <f>1.83*Q29/SUM($Q$29:$Q$30)</f>
+      <c r="B37" t="s">
+        <v>174</v>
+      </c>
+      <c r="C37" s="10">
+        <f>1.83*R29/SUM($R$29:$R$30)</f>
         <v>0.53910143272425248</v>
       </c>
-      <c r="C37" s="3">
+      <c r="D37" s="3">
         <f t="shared" si="18"/>
         <v>39.437587643434</v>
       </c>
-      <c r="D37" s="3">
+      <c r="E37" s="3">
         <f t="shared" si="19"/>
         <v>8.6866933135317179</v>
       </c>
-      <c r="E37" s="7">
+      <c r="F37" s="7">
         <f t="shared" si="15"/>
         <v>260.60079940595153</v>
       </c>
-      <c r="F37" s="8">
-        <v>4.54</v>
-      </c>
       <c r="G37" s="8">
         <v>4.54</v>
       </c>
       <c r="H37" s="8">
+        <v>4.54</v>
+      </c>
+      <c r="I37" s="8">
         <v>11.5</v>
       </c>
-      <c r="I37" s="3">
+      <c r="J37" s="3">
         <f t="shared" si="0"/>
         <v>0.20071286397934787</v>
       </c>
-      <c r="J37" s="8">
+      <c r="K37" s="8">
         <v>14.8</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B38" s="10">
-        <f>1.83*Q30/SUM($Q$29:$Q$30)</f>
+      <c r="B38" t="s">
+        <v>175</v>
+      </c>
+      <c r="C38" s="10">
+        <f>1.83*R30/SUM($R$29:$R$30)</f>
         <v>1.2908985672757476</v>
       </c>
-      <c r="C38" s="3">
+      <c r="D38" s="3">
         <f t="shared" si="18"/>
         <v>94.434780350066006</v>
       </c>
-      <c r="D38" s="3">
+      <c r="E38" s="3">
         <f t="shared" si="19"/>
         <v>18.589523690957876</v>
       </c>
-      <c r="E38" s="7">
+      <c r="F38" s="7">
         <f t="shared" si="15"/>
         <v>557.68571072873624</v>
       </c>
-      <c r="F38" s="8">
-        <v>5.08</v>
-      </c>
       <c r="G38" s="8">
         <v>5.08</v>
       </c>
       <c r="H38" s="8">
+        <v>5.08</v>
+      </c>
+      <c r="I38" s="8">
         <v>14.1</v>
       </c>
-      <c r="I38" s="3">
+      <c r="J38" s="3">
         <f t="shared" si="0"/>
         <v>0.24609142453120048</v>
       </c>
-      <c r="J38" s="8">
+      <c r="K38" s="8">
         <v>33.299999999999997</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="10">
-        <f>1.44*(Q15/SUM($Q$13:$Q$15))</f>
+      <c r="B39"/>
+      <c r="C39" s="10">
+        <f>1.44*(R15/SUM($R$13:$R$15))</f>
         <v>0.23522940863872555</v>
       </c>
-      <c r="C39" s="3">
+      <c r="D39" s="3">
         <f t="shared" si="18"/>
         <v>17.208042599003743</v>
       </c>
-      <c r="D39" s="3">
+      <c r="E39" s="3">
         <f t="shared" si="19"/>
         <v>2.1782332403802207</v>
       </c>
-      <c r="E39" s="7">
+      <c r="F39" s="7">
         <f t="shared" si="15"/>
         <v>65.346997211406617</v>
       </c>
-      <c r="F39" s="8">
-        <v>7.9</v>
-      </c>
       <c r="G39" s="8">
         <v>7.9</v>
       </c>
       <c r="H39" s="8">
+        <v>7.9</v>
+      </c>
+      <c r="I39" s="8">
         <v>13</v>
       </c>
-      <c r="I39" s="3">
+      <c r="J39" s="3">
         <f t="shared" si="0"/>
         <v>0.22689280275926285</v>
       </c>
-      <c r="J39" s="8">
+      <c r="K39" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B40" s="8">
+      <c r="B40" t="s">
+        <v>176</v>
+      </c>
+      <c r="C40" s="8">
         <v>0.61</v>
       </c>
-      <c r="C40" s="3">
-        <f t="shared" ref="C40:C57" si="20">B40/100*$O$5</f>
+      <c r="D40" s="3">
+        <f t="shared" ref="D40:D57" si="20">C40/100*$P$5</f>
         <v>44.624122664499993</v>
       </c>
-      <c r="D40" s="3">
-        <f t="shared" ref="D40:D53" si="21">C40/G40</f>
+      <c r="E40" s="3">
+        <f t="shared" ref="E40:E53" si="21">D40/H40</f>
         <v>17.163124101730766</v>
       </c>
-      <c r="E40" s="7">
-        <f t="shared" ref="E40:E53" si="22">D40*$O$2</f>
+      <c r="F40" s="7">
+        <f t="shared" ref="F40:F53" si="22">E40*$P$2</f>
         <v>514.89372305192296</v>
-      </c>
-      <c r="F40" s="8">
-        <v>2.6</v>
       </c>
       <c r="G40" s="8">
         <v>2.6</v>
       </c>
       <c r="H40" s="8">
+        <v>2.6</v>
+      </c>
+      <c r="I40" s="8">
         <v>10</v>
       </c>
-      <c r="I40" s="3">
+      <c r="J40" s="3">
         <f t="shared" si="0"/>
         <v>0.17453292519943295</v>
       </c>
-      <c r="J40" s="8">
+      <c r="K40" s="8">
         <v>11.5</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="8">
         <v>3.8</v>
       </c>
-      <c r="C41" s="3">
+      <c r="D41" s="3">
         <f t="shared" si="20"/>
         <v>277.98633790999997</v>
       </c>
-      <c r="D41" s="3">
+      <c r="E41" s="3">
         <f t="shared" si="21"/>
         <v>23.779840710863986</v>
       </c>
-      <c r="E41" s="7">
+      <c r="F41" s="7">
         <f t="shared" si="22"/>
         <v>713.39522132591958</v>
       </c>
-      <c r="F41" s="8">
-        <v>11.69</v>
-      </c>
       <c r="G41" s="8">
         <v>11.69</v>
       </c>
       <c r="H41" s="8">
+        <v>11.69</v>
+      </c>
+      <c r="I41" s="8">
         <v>10.7</v>
       </c>
-      <c r="I41" s="3">
+      <c r="J41" s="3">
         <f t="shared" si="0"/>
         <v>0.18675022996339324</v>
       </c>
-      <c r="J41" s="8">
+      <c r="K41" s="8">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="8">
+      <c r="B42"/>
+      <c r="C42" s="8">
         <v>0.45</v>
       </c>
-      <c r="C42" s="3">
+      <c r="D42" s="3">
         <f t="shared" si="20"/>
         <v>32.919434752500003</v>
       </c>
-      <c r="D42" s="3">
+      <c r="E42" s="3">
         <f t="shared" si="21"/>
         <v>6.0961916208333333</v>
       </c>
-      <c r="E42" s="7">
+      <c r="F42" s="7">
         <f t="shared" si="22"/>
         <v>182.88574862499999</v>
       </c>
-      <c r="F42" s="8">
-        <v>5.4</v>
-      </c>
       <c r="G42" s="8">
         <v>5.4</v>
       </c>
       <c r="H42" s="8">
+        <v>5.4</v>
+      </c>
+      <c r="I42" s="8">
         <v>0</v>
       </c>
-      <c r="I42" s="3">
+      <c r="J42" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J42" s="8">
+      <c r="K42" s="8">
         <v>2.4</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="8">
+      <c r="B43" t="s">
+        <v>178</v>
+      </c>
+      <c r="C43" s="8">
         <v>3.79</v>
       </c>
-      <c r="C43" s="3">
+      <c r="D43" s="3">
         <f t="shared" si="20"/>
         <v>277.25479491550004</v>
       </c>
-      <c r="D43" s="3">
+      <c r="E43" s="3">
         <f t="shared" si="21"/>
         <v>36.528958486890652</v>
       </c>
-      <c r="E43" s="7">
+      <c r="F43" s="7">
         <f t="shared" si="22"/>
         <v>1095.8687546067194</v>
       </c>
-      <c r="F43" s="8">
-        <v>7.59</v>
-      </c>
       <c r="G43" s="8">
         <v>7.59</v>
       </c>
       <c r="H43" s="8">
+        <v>7.59</v>
+      </c>
+      <c r="I43" s="8">
         <v>13.9</v>
       </c>
-      <c r="I43" s="3">
+      <c r="J43" s="3">
         <f t="shared" si="0"/>
         <v>0.24260076602721178</v>
       </c>
-      <c r="J43" s="11">
+      <c r="K43" s="11">
         <v>34.6</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B44" s="8">
+      <c r="B44" t="s">
+        <v>179</v>
+      </c>
+      <c r="C44" s="8">
         <v>2.29</v>
       </c>
-      <c r="C44" s="3">
+      <c r="D44" s="3">
         <f t="shared" si="20"/>
         <v>167.52334574049999</v>
       </c>
-      <c r="D44" s="3">
+      <c r="E44" s="3">
         <f t="shared" si="21"/>
         <v>4.1569068421960296</v>
       </c>
-      <c r="E44" s="7">
+      <c r="F44" s="7">
         <f t="shared" si="22"/>
         <v>124.70720526588089</v>
       </c>
-      <c r="F44" s="8">
-        <v>40.299999999999997</v>
-      </c>
       <c r="G44" s="8">
         <v>40.299999999999997</v>
       </c>
       <c r="H44" s="8">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="I44" s="8">
         <v>1.3</v>
       </c>
-      <c r="I44" s="3">
+      <c r="J44" s="3">
         <f t="shared" si="0"/>
         <v>2.2689280275926284E-2</v>
       </c>
-      <c r="J44" s="8">
+      <c r="K44" s="8">
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="8">
+      <c r="B45" t="s">
+        <v>180</v>
+      </c>
+      <c r="C45" s="8">
         <v>3.46</v>
       </c>
-      <c r="C45" s="3">
+      <c r="D45" s="3">
         <f t="shared" si="20"/>
         <v>253.11387609699997</v>
       </c>
-      <c r="D45" s="3">
+      <c r="E45" s="3">
         <f t="shared" si="21"/>
         <v>36.683170448840571</v>
       </c>
-      <c r="E45" s="7">
+      <c r="F45" s="7">
         <f t="shared" si="22"/>
         <v>1100.4951134652172</v>
       </c>
-      <c r="F45" s="8">
-        <v>6.9</v>
-      </c>
       <c r="G45" s="8">
         <v>6.9</v>
       </c>
       <c r="H45" s="8">
+        <v>6.9</v>
+      </c>
+      <c r="I45" s="8">
         <v>15.1</v>
       </c>
-      <c r="I45" s="3">
+      <c r="J45" s="3">
         <f t="shared" si="0"/>
         <v>0.26354471705114374</v>
       </c>
-      <c r="J45" s="8">
+      <c r="K45" s="8">
         <v>37.799999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B46" s="8">
+      <c r="B46" t="s">
+        <v>181</v>
+      </c>
+      <c r="C46" s="8">
         <v>2.6</v>
       </c>
-      <c r="C46" s="3">
+      <c r="D46" s="3">
         <f t="shared" si="20"/>
         <v>190.20117857000002</v>
       </c>
-      <c r="D46" s="3">
+      <c r="E46" s="3">
         <f t="shared" si="21"/>
         <v>9.8549833455958566</v>
       </c>
-      <c r="E46" s="7">
+      <c r="F46" s="7">
         <f t="shared" si="22"/>
         <v>295.6495003678757</v>
       </c>
-      <c r="F46" s="8">
-        <v>19.3</v>
-      </c>
       <c r="G46" s="8">
         <v>19.3</v>
       </c>
       <c r="H46" s="8">
+        <v>19.3</v>
+      </c>
+      <c r="I46" s="8">
         <v>12.9</v>
       </c>
-      <c r="I46" s="3">
+      <c r="J46" s="3">
         <f t="shared" si="0"/>
         <v>0.22514747350726852</v>
       </c>
-      <c r="J46" s="8">
+      <c r="K46" s="8">
         <v>24.5</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="8">
+      <c r="B47" t="s">
+        <v>182</v>
+      </c>
+      <c r="C47" s="8">
         <v>6.21</v>
       </c>
-      <c r="C47" s="3">
+      <c r="D47" s="3">
         <f t="shared" si="20"/>
         <v>454.28819958450003</v>
       </c>
-      <c r="D47" s="3">
+      <c r="E47" s="3">
         <f t="shared" si="21"/>
         <v>103.24731808738636</v>
       </c>
-      <c r="E47" s="7">
+      <c r="F47" s="7">
         <f t="shared" si="22"/>
         <v>3097.4195426215911</v>
       </c>
-      <c r="F47" s="8">
-        <v>4.4000000000000004</v>
-      </c>
       <c r="G47" s="8">
         <v>4.4000000000000004</v>
       </c>
       <c r="H47" s="8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I47" s="8">
         <v>28.3</v>
       </c>
-      <c r="I47" s="3">
+      <c r="J47" s="3">
         <f t="shared" si="0"/>
         <v>0.49392817831439528</v>
       </c>
-      <c r="J47" s="8">
+      <c r="K47" s="8">
         <v>28.2</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B48" s="8">
+      <c r="B48" t="s">
+        <v>183</v>
+      </c>
+      <c r="C48" s="8">
         <v>0.89</v>
       </c>
-      <c r="C48" s="3">
+      <c r="D48" s="3">
         <f t="shared" si="20"/>
         <v>65.107326510500002</v>
       </c>
-      <c r="D48" s="3">
+      <c r="E48" s="3">
         <f t="shared" si="21"/>
         <v>6.8534027905789472</v>
       </c>
-      <c r="E48" s="7">
+      <c r="F48" s="7">
         <f t="shared" si="22"/>
         <v>205.60208371736843</v>
       </c>
-      <c r="F48" s="8">
-        <v>9.5</v>
-      </c>
       <c r="G48" s="8">
         <v>9.5</v>
       </c>
       <c r="H48" s="8">
+        <v>9.5</v>
+      </c>
+      <c r="I48" s="8">
         <v>3</v>
       </c>
-      <c r="I48" s="3">
+      <c r="J48" s="3">
         <f t="shared" si="0"/>
         <v>5.2359877559829883E-2</v>
       </c>
-      <c r="J48" s="8">
+      <c r="K48" s="8">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" t="s">
+        <v>184</v>
+      </c>
+      <c r="C49" s="8">
         <v>1.91</v>
       </c>
-      <c r="C49" s="3">
+      <c r="D49" s="3">
         <f t="shared" si="20"/>
         <v>139.72471194949998</v>
       </c>
-      <c r="D49" s="3">
+      <c r="E49" s="3">
         <f t="shared" si="21"/>
         <v>20.457498089238648</v>
       </c>
-      <c r="E49" s="7">
+      <c r="F49" s="7">
         <f t="shared" si="22"/>
         <v>613.72494267715945</v>
       </c>
-      <c r="F49" s="8">
-        <v>6.83</v>
-      </c>
       <c r="G49" s="8">
         <v>6.83</v>
       </c>
       <c r="H49" s="8">
+        <v>6.83</v>
+      </c>
+      <c r="I49" s="8">
         <v>9.6</v>
       </c>
-      <c r="I49" s="3">
+      <c r="J49" s="3">
         <f t="shared" si="0"/>
         <v>0.16755160819145562</v>
       </c>
-      <c r="J49" s="8">
+      <c r="K49" s="8">
         <v>24.1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B50" t="s">
+        <v>185</v>
+      </c>
+      <c r="C50" s="8">
         <v>1.49</v>
       </c>
-      <c r="C50" s="3">
+      <c r="D50" s="3">
         <f t="shared" si="20"/>
         <v>108.99990618050001</v>
       </c>
-      <c r="D50" s="3">
+      <c r="E50" s="3">
         <f t="shared" si="21"/>
         <v>28.835954016005292</v>
       </c>
-      <c r="E50" s="7">
+      <c r="F50" s="7">
         <f t="shared" si="22"/>
         <v>865.07862048015875</v>
       </c>
-      <c r="F50" s="8">
-        <v>3.78</v>
-      </c>
       <c r="G50" s="8">
         <v>3.78</v>
       </c>
       <c r="H50" s="8">
+        <v>3.78</v>
+      </c>
+      <c r="I50" s="8">
         <v>13.7</v>
       </c>
-      <c r="I50" s="3">
+      <c r="J50" s="3">
         <f t="shared" si="0"/>
         <v>0.23911010752322312</v>
       </c>
-      <c r="J50" s="8">
+      <c r="K50" s="8">
         <v>28.2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B51" s="8">
+      <c r="B51" t="s">
+        <v>186</v>
+      </c>
+      <c r="C51" s="8">
         <v>3.84</v>
       </c>
-      <c r="C51" s="3">
+      <c r="D51" s="3">
         <f t="shared" si="20"/>
         <v>280.91250988799999</v>
       </c>
-      <c r="D51" s="3">
+      <c r="E51" s="3">
         <f t="shared" si="21"/>
         <v>28.289275920241693</v>
       </c>
-      <c r="E51" s="7">
+      <c r="F51" s="7">
         <f t="shared" si="22"/>
         <v>848.67827760725072</v>
       </c>
-      <c r="F51" s="8">
-        <v>9.93</v>
-      </c>
       <c r="G51" s="8">
         <v>9.93</v>
       </c>
       <c r="H51" s="8">
+        <v>9.93</v>
+      </c>
+      <c r="I51" s="8">
         <v>4.5</v>
       </c>
-      <c r="I51" s="3">
+      <c r="J51" s="3">
         <f t="shared" si="0"/>
         <v>7.8539816339744828E-2</v>
       </c>
-      <c r="J51" s="11">
+      <c r="K51" s="11">
         <v>10.6</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="8">
+      <c r="B52" t="s">
+        <v>187</v>
+      </c>
+      <c r="C52" s="8">
         <v>11.66</v>
       </c>
-      <c r="C52" s="3">
+      <c r="D52" s="3">
         <f t="shared" si="20"/>
         <v>852.97913158699998</v>
       </c>
-      <c r="D52" s="3">
+      <c r="E52" s="3">
         <f t="shared" si="21"/>
         <v>85.812789898088539</v>
       </c>
-      <c r="E52" s="7">
+      <c r="F52" s="7">
         <f t="shared" si="22"/>
         <v>2574.3836969426561</v>
       </c>
-      <c r="F52" s="8">
-        <v>9.94</v>
-      </c>
       <c r="G52" s="8">
         <v>9.94</v>
       </c>
       <c r="H52" s="8">
+        <v>9.94</v>
+      </c>
+      <c r="I52" s="8">
         <v>18.399999999999999</v>
       </c>
-      <c r="I52" s="3">
+      <c r="J52" s="3">
         <f t="shared" si="0"/>
         <v>0.32114058236695658</v>
       </c>
-      <c r="J52" s="11">
+      <c r="K52" s="11">
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" t="s">
+        <v>188</v>
+      </c>
+      <c r="C53" s="8">
         <v>6.06</v>
       </c>
-      <c r="C53" s="3">
+      <c r="D53" s="3">
         <f t="shared" si="20"/>
         <v>443.31505466699997</v>
       </c>
-      <c r="D53" s="3">
+      <c r="E53" s="3">
         <f t="shared" si="21"/>
         <v>45.797009779648761</v>
       </c>
-      <c r="E53" s="7">
+      <c r="F53" s="7">
         <f t="shared" si="22"/>
         <v>1373.9102933894628</v>
       </c>
-      <c r="F53" s="8">
-        <v>9.68</v>
-      </c>
       <c r="G53" s="8">
         <v>9.68</v>
       </c>
       <c r="H53" s="8">
+        <v>9.68</v>
+      </c>
+      <c r="I53" s="8">
         <v>29.6</v>
       </c>
-      <c r="I53" s="3">
+      <c r="J53" s="3">
         <f t="shared" si="0"/>
         <v>0.51661745859032149</v>
       </c>
-      <c r="J53" s="11">
+      <c r="K53" s="11">
         <v>11.2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="23">
+      <c r="B54" s="22"/>
+      <c r="C54" s="23">
         <v>0.76</v>
       </c>
-      <c r="C54" s="3">
+      <c r="D54" s="3">
         <f t="shared" si="20"/>
         <v>55.597267582000001</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="23">
+      <c r="B55" s="22"/>
+      <c r="C55" s="23">
         <v>0.38</v>
       </c>
-      <c r="C55" s="3">
+      <c r="D55" s="3">
         <f t="shared" si="20"/>
         <v>27.798633791</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="B56" s="23">
+      <c r="B56" s="22"/>
+      <c r="C56" s="23">
         <v>0.23</v>
       </c>
-      <c r="C56" s="3">
+      <c r="D56" s="3">
         <f t="shared" si="20"/>
         <v>16.825488873499999</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B57" s="23">
+      <c r="B57" s="22"/>
+      <c r="C57" s="23">
         <v>0.33</v>
       </c>
-      <c r="C57" s="3">
+      <c r="D57" s="3">
         <f t="shared" si="20"/>
         <v>24.140918818499998</v>
       </c>
@@ -5343,8 +5596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>